<commit_message>
some stuff but I am tired so I am taking a break
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\samsat-quiz-app\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\samsat-quiz-app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B820EF-1D75-463A-9141-F6AA823F30C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787E716A-2993-4E7E-AB6E-80B999FA9E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24300" yWindow="1785" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Debug" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="13">
   <si>
     <t>Question</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>Hint</t>
   </si>
 </sst>
 </file>
@@ -390,19 +393,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -421,8 +424,11 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -438,11 +444,14 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -458,11 +467,14 @@
       <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -478,11 +490,14 @@
       <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -498,11 +513,14 @@
       <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -518,11 +536,14 @@
       <c r="E6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -538,7 +559,10 @@
       <c r="E7" t="s">
         <v>11</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
         <v>2</v>
       </c>
     </row>
@@ -555,9 +579,9 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -586,13 +610,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93C1C905-5E3D-4F98-83EA-1A1AC8B7A352}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
font and reference images
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\samsat-quiz-app\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\samsat-quiz-app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787E716A-2993-4E7E-AB6E-80B999FA9E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C391AAE5-5BDD-49AA-901C-2C76A5C9F81C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-3015" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Debug" sheetId="1" r:id="rId1"/>
@@ -37,20 +37,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
   <si>
     <t>Question</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>Correct</t>
   </si>
   <si>
@@ -72,10 +63,31 @@
     <t>How?</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
     <t>Hint</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Maybe</t>
+  </si>
+  <si>
+    <t>So</t>
+  </si>
+  <si>
+    <t>Someone</t>
+  </si>
+  <si>
+    <t>Else</t>
+  </si>
+  <si>
+    <t>Is</t>
+  </si>
+  <si>
+    <t>Ugly</t>
   </si>
 </sst>
 </file>
@@ -396,16 +408,16 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -422,28 +434,28 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
       <c r="F2">
         <v>1</v>
       </c>
@@ -451,18 +463,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -474,21 +486,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -497,21 +509,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -520,21 +532,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -543,21 +555,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F7">
         <v>2</v>
@@ -579,9 +591,9 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -598,7 +610,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -614,9 +626,9 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -633,7 +645,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
styles and documentation and refactoring
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -5,17 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\samsat-quiz-app\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\samsat-quiz-app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C391AAE5-5BDD-49AA-901C-2C76A5C9F81C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2F3DE4-7D57-41C4-B82F-4D35E22040F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3015" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Debug" sheetId="1" r:id="rId1"/>
-    <sheet name="Quiz1" sheetId="2" r:id="rId2"/>
-    <sheet name="Quiz2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
   <si>
     <t>Question</t>
   </si>
@@ -88,6 +86,18 @@
   </si>
   <si>
     <t>Ugly</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>Some Answer</t>
+  </si>
+  <si>
+    <t>An Interesting Answer</t>
+  </si>
+  <si>
+    <t>An incorrect answer for some stuff</t>
   </si>
 </sst>
 </file>
@@ -405,19 +415,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,7 +452,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -463,7 +475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -486,7 +498,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -509,7 +521,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -532,7 +544,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -555,7 +567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -578,73 +590,26 @@
         <v>2</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F6E16CF-BF9E-43CD-82E7-EA9567C3AE6F}">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93C1C905-5E3D-4F98-83EA-1A1AC8B7A352}">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
         <v>1</v>
       </c>
     </row>

</xml_diff>